<commit_message>
s is update for the past
</commit_message>
<xml_diff>
--- a/EngineModel/Model Parameters_ScaniaDC12.xlsx
+++ b/EngineModel/Model Parameters_ScaniaDC12.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-12" windowWidth="6780" windowHeight="4596" firstSheet="7" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="-12" windowWidth="6780" windowHeight="4596" firstSheet="9" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet5" sheetId="9" r:id="rId1"/>
@@ -31,7 +31,7 @@
     <sheet name="Friction" sheetId="19" r:id="rId17"/>
     <sheet name="Valve" sheetId="20" r:id="rId18"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -32050,8 +32050,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="32549647" y="7102928"/>
-          <a:ext cx="5148857" cy="7160626"/>
+          <a:off x="32699078" y="7116783"/>
+          <a:ext cx="5172608" cy="7404069"/>
           <a:chOff x="32954980" y="6883293"/>
           <a:chExt cx="5025912" cy="6451773"/>
         </a:xfrm>
@@ -33117,14 +33117,14 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>241147</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>124650</xdr:rowOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>125506</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
       <xdr:colOff>89662</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>116262</xdr:rowOff>
+      <xdr:rowOff>89648</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -33147,8 +33147,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8134991" y="696150"/>
-          <a:ext cx="7742359" cy="8754612"/>
+          <a:off x="8165947" y="842682"/>
+          <a:ext cx="7773315" cy="8032378"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -33266,6 +33266,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -33301,6 +33318,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -35157,8 +35191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH42"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="W9" sqref="W9"/>
+    <sheetView showWhiteSpace="0" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -36256,27 +36290,27 @@
     </row>
     <row r="15" spans="1:26">
       <c r="L15">
-        <f>L4*$C4</f>
+        <f t="shared" ref="L15:Q15" si="2">L4*$C4</f>
         <v>191535.42709885415</v>
       </c>
       <c r="M15">
-        <f>M4*$C4</f>
+        <f t="shared" si="2"/>
         <v>175574.14150728303</v>
       </c>
       <c r="N15">
-        <f>N4*$C4</f>
+        <f t="shared" si="2"/>
         <v>159612.85591571181</v>
       </c>
       <c r="O15">
-        <f>O4*$C4</f>
+        <f t="shared" si="2"/>
         <v>143651.5703241406</v>
       </c>
       <c r="P15">
-        <f>P4*$C4</f>
+        <f t="shared" si="2"/>
         <v>127690.28473256946</v>
       </c>
       <c r="Q15">
-        <f>Q4*$C4</f>
+        <f t="shared" si="2"/>
         <v>111728.99914099825</v>
       </c>
       <c r="T15">
@@ -36292,27 +36326,27 @@
     </row>
     <row r="16" spans="1:26">
       <c r="L16">
-        <f>L6*$C6</f>
+        <f t="shared" ref="L16:Q16" si="3">L6*$C6</f>
         <v>170253.71297675924</v>
       </c>
       <c r="M16">
-        <f>M6*$C6</f>
+        <f t="shared" si="3"/>
         <v>156065.90356202936</v>
       </c>
       <c r="N16">
-        <f>N6*$C6</f>
+        <f t="shared" si="3"/>
         <v>141878.09414729939</v>
       </c>
       <c r="O16">
-        <f>O6*$C6</f>
+        <f t="shared" si="3"/>
         <v>127690.28473256945</v>
       </c>
       <c r="P16">
-        <f>P6*$C6</f>
+        <f t="shared" si="3"/>
         <v>113502.4753178395</v>
       </c>
       <c r="Q16">
-        <f>Q6*$C6</f>
+        <f t="shared" si="3"/>
         <v>99314.665903109591</v>
       </c>
       <c r="T16">
@@ -36332,27 +36366,27 @@
         <v>223457.99828199649</v>
       </c>
       <c r="L17">
-        <f>L8*$C8</f>
+        <f t="shared" ref="L17:Q17" si="4">L8*$C8</f>
         <v>148971.99885466433</v>
       </c>
       <c r="M17">
-        <f>M8*$C8</f>
+        <f t="shared" si="4"/>
         <v>136557.66561677563</v>
       </c>
       <c r="N17">
-        <f>N8*$C8</f>
+        <f t="shared" si="4"/>
         <v>124143.33237888696</v>
       </c>
       <c r="O17">
-        <f>O8*$C8</f>
+        <f t="shared" si="4"/>
         <v>111728.99914099825</v>
       </c>
       <c r="P17">
-        <f>P8*$C8</f>
+        <f t="shared" si="4"/>
         <v>99314.665903109577</v>
       </c>
       <c r="Q17">
-        <f>Q8*$C8</f>
+        <f t="shared" si="4"/>
         <v>86900.332665220849</v>
       </c>
       <c r="T17">
@@ -36372,27 +36406,27 @@
         <v>191535.42709885415</v>
       </c>
       <c r="L18">
-        <f>L10*$C10</f>
+        <f t="shared" ref="L18:Q18" si="5">L10*$C10</f>
         <v>127690.28473256945</v>
       </c>
       <c r="M18">
-        <f>M10*$C10</f>
+        <f t="shared" si="5"/>
         <v>117049.427671522</v>
       </c>
       <c r="N18">
-        <f>N10*$C10</f>
+        <f t="shared" si="5"/>
         <v>106408.57061047453</v>
       </c>
       <c r="O18">
-        <f>O10*$C10</f>
+        <f t="shared" si="5"/>
         <v>95767.713549427077</v>
       </c>
       <c r="P18">
-        <f>P10*$C10</f>
+        <f t="shared" si="5"/>
         <v>85126.856488379635</v>
       </c>
       <c r="Q18">
-        <f>Q10*$C10</f>
+        <f t="shared" si="5"/>
         <v>74485.999427332179</v>
       </c>
       <c r="T18">
@@ -36408,31 +36442,31 @@
     </row>
     <row r="19" spans="2:26">
       <c r="L19">
-        <f t="shared" ref="L19:T19" si="2">L12*$C12</f>
+        <f t="shared" ref="L19:T19" si="6">L12*$C12</f>
         <v>106408.57061047453</v>
       </c>
       <c r="M19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>97541.189726268334</v>
       </c>
       <c r="N19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>88673.808842062121</v>
       </c>
       <c r="O19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>79806.427957855893</v>
       </c>
       <c r="P19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>70939.047073649708</v>
       </c>
       <c r="Q19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>62071.66618944348</v>
       </c>
       <c r="T19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>35469.523536824854</v>
       </c>
       <c r="Y19" s="32">
@@ -37712,8 +37746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -38800,7 +38834,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="U23" sqref="U23:AB44"/>
+      <selection pane="bottomRight" activeCell="AC13" sqref="AC13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8"/>
@@ -44566,7 +44600,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BW28"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -54129,11 +54163,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CA24"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="AV16" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="S3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="BE54" sqref="BE54"/>
+      <selection pane="bottomRight" activeCell="AS64" sqref="AS64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8"/>
@@ -65039,11 +65073,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CC23"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="BR3" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="CE18" sqref="CE18"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8"/>
@@ -68798,8 +68832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G82"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="X17" sqref="X17"/>
+    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>